<commit_message>
auto upload image with dev
</commit_message>
<xml_diff>
--- a/azota_assets/medias/de_mau_azota_excel.xlsx
+++ b/azota_assets/medias/de_mau_azota_excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nguyenvantuan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nguyenvantuan/sources/azota/frontend.azota1/core/ClientApp/src/assets/medias/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822BF9D2-3E1D-9A48-841B-2A7BD161101A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF379A1-3EE8-C244-9B99-26BEB3970AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="54">
-  <si>
-    <t>Đề\câu</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="52">
   <si>
     <t>1</t>
   </si>
@@ -145,9 +142,6 @@
     <t>40</t>
   </si>
   <si>
-    <t>000</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -160,9 +154,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>101</t>
-  </si>
-  <si>
     <t>102</t>
   </si>
   <si>
@@ -182,6 +173,9 @@
   </si>
   <si>
     <t>108</t>
+  </si>
+  <si>
+    <t>Mã đề\câu</t>
   </si>
 </sst>
 </file>
@@ -594,742 +588,742 @@
   <dimension ref="A1:AO10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="41" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:41" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>42</v>
+      <c r="A2" s="3">
+        <v>101</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:41" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AH3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AL3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AO3" s="3" t="s">
-        <v>45</v>
+      <c r="B3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:41" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>43</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>42</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="V4" s="2" t="s">
         <v>42</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AG4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AH4" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="AI4" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="AJ4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AK4" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="AL4" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AM4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AN4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AO4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:41" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>42</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="AD5" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AG5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AH5" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AJ5" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>42</v>
       </c>
       <c r="AL5" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AM5" s="2" t="s">
         <v>42</v>
       </c>
       <c r="AN5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AO5" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:41" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>43</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R6" s="2" t="s">
         <v>43</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="T6" s="2" t="s">
         <v>42</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="W6" s="2" t="s">
         <v>43</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="Z6" s="2" t="s">
         <v>43</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AB6" s="2" t="s">
         <v>43</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AD6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AE6" s="2" t="s">
         <v>42</v>
       </c>
       <c r="AF6" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AG6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AH6" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AI6" s="2" t="s">
         <v>42</v>
@@ -1338,27 +1332,27 @@
         <v>42</v>
       </c>
       <c r="AK6" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AL6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AM6" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AN6" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AO6" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:41" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>42</v>
@@ -1367,251 +1361,251 @@
         <v>42</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>42</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>42</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Y7" s="2" t="s">
         <v>42</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AA7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="AB7" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="AC7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AD7" s="2" t="s">
         <v>43</v>
       </c>
       <c r="AE7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AF7" s="2" t="s">
         <v>43</v>
       </c>
       <c r="AG7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="AH7" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="AI7" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="AJ7" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AK7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AL7" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="AM7" s="2" t="s">
         <v>42</v>
       </c>
       <c r="AN7" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AO7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:41" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="T8" s="2" t="s">
         <v>43</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AA8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AB8" s="2" t="s">
         <v>42</v>
       </c>
       <c r="AC8" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AD8" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="AE8" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="AF8" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="AG8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="AH8" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="AI8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AJ8" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AK8" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AL8" s="2" t="s">
         <v>43</v>
       </c>
       <c r="AM8" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AN8" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="AO8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:41" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>42</v>
@@ -1620,237 +1614,237 @@
         <v>43</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="W9" s="2" t="s">
         <v>43</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Y9" s="2" t="s">
         <v>43</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="AA9" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AE9" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AF9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AG9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AH9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AI9" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AJ9" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AK9" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="AL9" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="AM9" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AN9" s="2" t="s">
         <v>42</v>
       </c>
       <c r="AO9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:41" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AE10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AG10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AH10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="AI10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AJ10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="AK10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AL10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AM10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AN10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AO10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>